<commit_message>
Change Colab notebook name
</commit_message>
<xml_diff>
--- a/preprocessing/workshop_feature_selection.xlsx
+++ b/preprocessing/workshop_feature_selection.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\agile2024_rf_interpretability\preprocessing\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D61A9627-60B8-44B4-A513-CF7E2BA61788}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="workshop_feature_selection" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -370,8 +376,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -434,13 +440,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -478,7 +492,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -512,6 +526,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -546,9 +561,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -721,20 +737,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G83"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="28.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="7" width="27.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="7" width="27.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -757,7 +773,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -765,22 +781,22 @@
         <v>89</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D2">
-        <v>0.1830954195286399</v>
+        <v>0.18309541952863989</v>
       </c>
       <c r="E2">
         <v>0.2401939071570538</v>
       </c>
       <c r="F2">
-        <v>0.2499323404781947</v>
+        <v>0.24993234047819471</v>
       </c>
       <c r="G2">
         <v>0.2800029289833102</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -788,10 +804,10 @@
         <v>89</v>
       </c>
       <c r="C3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -799,10 +815,10 @@
         <v>89</v>
       </c>
       <c r="C4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -810,10 +826,10 @@
         <v>89</v>
       </c>
       <c r="C5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -821,22 +837,22 @@
         <v>11</v>
       </c>
       <c r="C6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D6">
-        <v>0.0152116651505534</v>
+        <v>1.5211665150553401E-2</v>
       </c>
       <c r="E6">
-        <v>0.0134421585240059</v>
+        <v>1.34421585240059E-2</v>
       </c>
       <c r="F6">
-        <v>0.0176455617321082</v>
+        <v>1.7645561732108201E-2</v>
       </c>
       <c r="G6">
-        <v>0.0303367296492013</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
+        <v>3.03367296492013E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -844,22 +860,22 @@
         <v>90</v>
       </c>
       <c r="C7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D7">
-        <v>0.0115162565702646</v>
+        <v>1.15162565702646E-2</v>
       </c>
       <c r="E7">
-        <v>0.0214553545636356</v>
+        <v>2.1455354563635599E-2</v>
       </c>
       <c r="F7">
-        <v>0.0198817355363302</v>
+        <v>1.98817355363302E-2</v>
       </c>
       <c r="G7">
-        <v>0.0303413699923845</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
+        <v>3.0341369992384501E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -867,22 +883,22 @@
         <v>90</v>
       </c>
       <c r="C8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D8">
-        <v>0.0176537329642707</v>
+        <v>1.76537329642707E-2</v>
       </c>
       <c r="E8">
-        <v>0.0228666650848857</v>
+        <v>2.28666650848857E-2</v>
       </c>
       <c r="F8">
-        <v>0.0362103557280772</v>
+        <v>3.6210355728077202E-2</v>
       </c>
       <c r="G8">
-        <v>0.0242820285420161</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
+        <v>2.4282028542016099E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -890,19 +906,19 @@
         <v>90</v>
       </c>
       <c r="C9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D9">
-        <v>0.0103508968883411</v>
+        <v>1.03508968883411E-2</v>
       </c>
       <c r="E9">
-        <v>0.0194781329905299</v>
+        <v>1.94781329905299E-2</v>
       </c>
       <c r="F9">
-        <v>0.022232376666281</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
+        <v>2.2232376666281001E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>15</v>
       </c>
@@ -910,22 +926,22 @@
         <v>90</v>
       </c>
       <c r="C10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D10">
-        <v>0.0043120462299322</v>
+        <v>4.3120462299322E-3</v>
       </c>
       <c r="E10">
-        <v>0.0115097664845701</v>
+        <v>1.15097664845701E-2</v>
       </c>
       <c r="F10">
-        <v>0.0171115928678321</v>
+        <v>1.71115928678321E-2</v>
       </c>
       <c r="G10">
-        <v>0.0198432673781565</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7">
+        <v>1.98432673781565E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>16</v>
       </c>
@@ -933,22 +949,22 @@
         <v>91</v>
       </c>
       <c r="C11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D11">
-        <v>0.0096982864771144</v>
+        <v>9.6982864771144005E-3</v>
       </c>
       <c r="E11">
-        <v>0.0210422700052141</v>
+        <v>2.1042270005214098E-2</v>
       </c>
       <c r="F11">
-        <v>0.0109172723811547</v>
+        <v>1.09172723811547E-2</v>
       </c>
       <c r="G11">
-        <v>0.0170759407519888</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7">
+        <v>1.7075940751988799E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>17</v>
       </c>
@@ -956,10 +972,10 @@
         <v>91</v>
       </c>
       <c r="C12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>18</v>
       </c>
@@ -967,10 +983,10 @@
         <v>91</v>
       </c>
       <c r="C13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>19</v>
       </c>
@@ -978,10 +994,10 @@
         <v>91</v>
       </c>
       <c r="C14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>20</v>
       </c>
@@ -989,22 +1005,22 @@
         <v>92</v>
       </c>
       <c r="C15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D15">
-        <v>0.0014317221485484</v>
+        <v>1.4317221485484E-3</v>
       </c>
       <c r="E15">
-        <v>0.0037503382779156</v>
+        <v>3.7503382779156E-3</v>
       </c>
       <c r="F15">
-        <v>0.0032593964031672</v>
+        <v>3.2593964031672001E-3</v>
       </c>
       <c r="G15">
-        <v>0.0063184461487259</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7">
+        <v>6.3184461487258998E-3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>21</v>
       </c>
@@ -1012,10 +1028,10 @@
         <v>92</v>
       </c>
       <c r="C16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>22</v>
       </c>
@@ -1023,10 +1039,10 @@
         <v>92</v>
       </c>
       <c r="C17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>23</v>
       </c>
@@ -1034,10 +1050,10 @@
         <v>92</v>
       </c>
       <c r="C18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>24</v>
       </c>
@@ -1045,22 +1061,22 @@
         <v>93</v>
       </c>
       <c r="C19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D19">
-        <v>0.0172766059004018</v>
+        <v>1.7276605900401799E-2</v>
       </c>
       <c r="E19">
-        <v>0.0832047914917587</v>
+        <v>8.3204791491758703E-2</v>
       </c>
       <c r="F19">
-        <v>0.0332280477872549</v>
+        <v>3.3228047787254897E-2</v>
       </c>
       <c r="G19">
-        <v>0.0520097380405032</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7">
+        <v>5.2009738040503198E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>25</v>
       </c>
@@ -1068,13 +1084,13 @@
         <v>93</v>
       </c>
       <c r="C20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D20">
-        <v>0.0172250108218917</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7">
+        <v>1.7225010821891699E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>26</v>
       </c>
@@ -1082,16 +1098,16 @@
         <v>93</v>
       </c>
       <c r="C21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D21">
-        <v>0.06693712058306441</v>
+        <v>6.6937120583064405E-2</v>
       </c>
       <c r="E21">
-        <v>0.0527464176850245</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7">
+        <v>5.2746417685024499E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>27</v>
       </c>
@@ -1099,19 +1115,19 @@
         <v>93</v>
       </c>
       <c r="C22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D22">
-        <v>0.0146835336343972</v>
+        <v>1.46835336343972E-2</v>
       </c>
       <c r="E22">
-        <v>0.040751355771573</v>
+        <v>4.0751355771573003E-2</v>
       </c>
       <c r="F22">
-        <v>0.0343590058984972</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7">
+        <v>3.4359005898497198E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>28</v>
       </c>
@@ -1119,7 +1135,7 @@
         <v>94</v>
       </c>
       <c r="C23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D23">
         <v>0</v>
@@ -1134,7 +1150,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:7">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>29</v>
       </c>
@@ -1142,16 +1158,16 @@
         <v>94</v>
       </c>
       <c r="C24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D24">
-        <v>0.0093178929953102</v>
+        <v>9.3178929953102001E-3</v>
       </c>
       <c r="E24">
-        <v>0.0178851835589719</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7">
+        <v>1.7885183558971899E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>30</v>
       </c>
@@ -1159,16 +1175,16 @@
         <v>94</v>
       </c>
       <c r="C25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D25">
-        <v>0.09535075595865521</v>
+        <v>9.5350755958655206E-2</v>
       </c>
       <c r="E25">
-        <v>0.1433876538301826</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7">
+        <v>0.14338765383018259</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>31</v>
       </c>
@@ -1176,10 +1192,10 @@
         <v>94</v>
       </c>
       <c r="C26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>32</v>
       </c>
@@ -1187,13 +1203,13 @@
         <v>95</v>
       </c>
       <c r="C27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D27">
-        <v>0.016771734635242</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7">
+        <v>1.6771734635242001E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>33</v>
       </c>
@@ -1201,13 +1217,13 @@
         <v>95</v>
       </c>
       <c r="C28">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D28">
-        <v>0.0361069421912022</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7">
+        <v>3.6106942191202203E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>34</v>
       </c>
@@ -1215,22 +1231,22 @@
         <v>95</v>
       </c>
       <c r="C29">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D29">
-        <v>0.0166906014060951</v>
+        <v>1.6690601406095101E-2</v>
       </c>
       <c r="E29">
-        <v>0.0358543878858999</v>
+        <v>3.5854387885899897E-2</v>
       </c>
       <c r="F29">
-        <v>0.0284217958028845</v>
+        <v>2.8421795802884502E-2</v>
       </c>
       <c r="G29">
-        <v>0.035725017699336</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7">
+        <v>3.5725017699335997E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>35</v>
       </c>
@@ -1238,22 +1254,22 @@
         <v>96</v>
       </c>
       <c r="C30">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D30">
-        <v>0.05386018953892</v>
+        <v>5.3860189538920002E-2</v>
       </c>
       <c r="E30">
-        <v>0.07065294175245521</v>
+        <v>7.0652941752455206E-2</v>
       </c>
       <c r="F30">
-        <v>0.0273136797251055</v>
+        <v>2.73136797251055E-2</v>
       </c>
       <c r="G30">
-        <v>0.08551168284374459</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7">
+        <v>8.5511682843744594E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>36</v>
       </c>
@@ -1261,22 +1277,22 @@
         <v>97</v>
       </c>
       <c r="C31">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D31">
-        <v>0.0149626750654914</v>
+        <v>1.49626750654914E-2</v>
       </c>
       <c r="E31">
-        <v>0.0148671667706427</v>
+        <v>1.48671667706427E-2</v>
       </c>
       <c r="F31">
-        <v>0.010092100038952</v>
+        <v>1.0092100038951999E-2</v>
       </c>
       <c r="G31">
-        <v>0.0182469801571589</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7">
+        <v>1.82469801571589E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>37</v>
       </c>
@@ -1284,16 +1300,16 @@
         <v>98</v>
       </c>
       <c r="C32">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D32">
-        <v>0.0104265387447988</v>
+        <v>1.04265387447988E-2</v>
       </c>
       <c r="E32">
-        <v>0.0068478568374244</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7">
+        <v>6.8478568374244E-3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>38</v>
       </c>
@@ -1301,16 +1317,16 @@
         <v>98</v>
       </c>
       <c r="C33">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D33">
         <v>0</v>
       </c>
       <c r="E33">
-        <v>0.0023376211328257</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7">
+        <v>2.3376211328256999E-3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>39</v>
       </c>
@@ -1318,22 +1334,22 @@
         <v>98</v>
       </c>
       <c r="C34">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D34">
         <v>0.1124311656140364</v>
       </c>
       <c r="E34">
-        <v>0.1755571520627406</v>
+        <v>0.17555715206274061</v>
       </c>
       <c r="F34">
         <v>0.1161012873723599</v>
       </c>
       <c r="G34">
-        <v>0.2119849936491588</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7">
+        <v>0.21198499364915879</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>40</v>
       </c>
@@ -1341,19 +1357,19 @@
         <v>98</v>
       </c>
       <c r="C35">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D35">
-        <v>0.0476636071798354</v>
+        <v>4.76636071798354E-2</v>
       </c>
       <c r="E35">
-        <v>0.0321423067864063</v>
+        <v>3.2142306786406297E-2</v>
       </c>
       <c r="F35">
-        <v>0.0839059871253382</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7">
+        <v>8.3905987125338199E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>41</v>
       </c>
@@ -1361,22 +1377,22 @@
         <v>99</v>
       </c>
       <c r="C36">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D36">
-        <v>0.0449470594771525</v>
+        <v>4.4947059477152503E-2</v>
       </c>
       <c r="E36">
-        <v>0.1463152720315719</v>
+        <v>0.14631527203157191</v>
       </c>
       <c r="F36">
-        <v>0.09481046684395029</v>
+        <v>9.4810466843950295E-2</v>
       </c>
       <c r="G36">
-        <v>0.1000506704142717</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7">
+        <v>0.10005067041427169</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>42</v>
       </c>
@@ -1384,22 +1400,22 @@
         <v>42</v>
       </c>
       <c r="C37">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D37">
-        <v>0.0446727918728388</v>
+        <v>4.4672791872838798E-2</v>
       </c>
       <c r="E37">
-        <v>0.0406009437983081</v>
+        <v>4.0600943798308101E-2</v>
       </c>
       <c r="F37">
-        <v>0.0789613382388774</v>
+        <v>7.8961338238877396E-2</v>
       </c>
       <c r="G37">
-        <v>0.0874521503874064</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7">
+        <v>8.7452150387406405E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>43</v>
       </c>
@@ -1407,10 +1423,10 @@
         <v>100</v>
       </c>
       <c r="C38">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>44</v>
       </c>
@@ -1418,22 +1434,22 @@
         <v>100</v>
       </c>
       <c r="C39">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D39">
-        <v>0.0235591082463387</v>
+        <v>2.3559108246338702E-2</v>
       </c>
       <c r="E39">
-        <v>0.0513095829007819</v>
+        <v>5.13095829007819E-2</v>
       </c>
       <c r="F39">
-        <v>0.0327593343247679</v>
+        <v>3.2759334324767901E-2</v>
       </c>
       <c r="G39">
-        <v>0.0354967414262427</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7">
+        <v>3.5496741426242699E-2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>45</v>
       </c>
@@ -1441,22 +1457,22 @@
         <v>101</v>
       </c>
       <c r="C40">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D40">
-        <v>0.0165037514534053</v>
+        <v>1.65037514534053E-2</v>
       </c>
       <c r="E40">
-        <v>0.0186408774618005</v>
+        <v>1.8640877461800501E-2</v>
       </c>
       <c r="F40">
-        <v>0.0209980354812055</v>
+        <v>2.0998035481205501E-2</v>
       </c>
       <c r="G40">
-        <v>0.0201944606483231</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7">
+        <v>2.0194460648323101E-2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>46</v>
       </c>
@@ -1464,19 +1480,19 @@
         <v>102</v>
       </c>
       <c r="C41">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D41">
-        <v>0.008432107704582499</v>
+        <v>8.4321077045824994E-3</v>
       </c>
       <c r="E41">
-        <v>0.0174984950830768</v>
+        <v>1.7498495083076802E-2</v>
       </c>
       <c r="F41">
-        <v>0.046457124619696</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7">
+        <v>4.6457124619695998E-2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>47</v>
       </c>
@@ -1484,13 +1500,13 @@
         <v>102</v>
       </c>
       <c r="C42">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D42">
-        <v>0.0111310141587837</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7">
+        <v>1.11310141587837E-2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>48</v>
       </c>
@@ -1498,22 +1514,22 @@
         <v>102</v>
       </c>
       <c r="C43">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D43">
-        <v>0.058887998848164</v>
+        <v>5.8887998848164001E-2</v>
       </c>
       <c r="E43">
-        <v>0.0384050168470202</v>
+        <v>3.8405016847020197E-2</v>
       </c>
       <c r="F43">
-        <v>0.0422959846641135</v>
+        <v>4.2295984664113502E-2</v>
       </c>
       <c r="G43">
-        <v>0.0834263027191052</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7">
+        <v>8.34263027191052E-2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>49</v>
       </c>
@@ -1521,16 +1537,16 @@
         <v>102</v>
       </c>
       <c r="C44">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D44">
-        <v>0.0429868066191573</v>
+        <v>4.2986806619157297E-2</v>
       </c>
       <c r="E44">
-        <v>0.0526641319528944</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7">
+        <v>5.2664131952894398E-2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>50</v>
       </c>
@@ -1538,22 +1554,22 @@
         <v>103</v>
       </c>
       <c r="C45">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D45">
-        <v>0.0094982254899232</v>
+        <v>9.4982254899232E-3</v>
       </c>
       <c r="E45">
-        <v>0.0478222852569401</v>
+        <v>4.78222852569401E-2</v>
       </c>
       <c r="F45">
-        <v>0.01504605806165</v>
+        <v>1.504605806165E-2</v>
       </c>
       <c r="G45">
-        <v>0.0479958682392835</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7">
+        <v>4.79958682392835E-2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>51</v>
       </c>
@@ -1561,22 +1577,22 @@
         <v>104</v>
       </c>
       <c r="C46">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D46">
-        <v>0.0833757163375249</v>
+        <v>8.3375716337524899E-2</v>
       </c>
       <c r="E46">
-        <v>0.0571100259804165</v>
+        <v>5.71100259804165E-2</v>
       </c>
       <c r="F46">
-        <v>0.0726587633454361</v>
+        <v>7.2658763345436098E-2</v>
       </c>
       <c r="G46">
-        <v>0.0617595953024032</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7">
+        <v>6.17595953024032E-2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>52</v>
       </c>
@@ -1584,19 +1600,19 @@
         <v>104</v>
       </c>
       <c r="C47">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D47">
         <v>0.1067460267881114</v>
       </c>
       <c r="E47">
-        <v>0.0959006450443583</v>
+        <v>9.5900645044358301E-2</v>
       </c>
       <c r="F47">
         <v>0.1283562056879857</v>
       </c>
     </row>
-    <row r="48" spans="1:7">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>53</v>
       </c>
@@ -1604,7 +1620,7 @@
         <v>105</v>
       </c>
       <c r="C48">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D48">
         <v>0</v>
@@ -1619,7 +1635,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:7">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>54</v>
       </c>
@@ -1627,22 +1643,22 @@
         <v>105</v>
       </c>
       <c r="C49">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D49">
         <v>0</v>
       </c>
       <c r="E49">
-        <v>0.0008123218615486</v>
+        <v>8.123218615486E-4</v>
       </c>
       <c r="F49">
-        <v>0.0004151398617415</v>
+        <v>4.1513986174150001E-4</v>
       </c>
       <c r="G49">
-        <v>0.0018320604376498</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7">
+        <v>1.8320604376498E-3</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>55</v>
       </c>
@@ -1650,13 +1666,13 @@
         <v>105</v>
       </c>
       <c r="C50">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D50">
         <v>0.1542914148622577</v>
       </c>
       <c r="E50">
-        <v>0.124884218537708</v>
+        <v>0.12488421853770799</v>
       </c>
       <c r="F50">
         <v>0.2362430405224723</v>
@@ -1665,7 +1681,7 @@
         <v>0.219420175818833</v>
       </c>
     </row>
-    <row r="51" spans="1:7">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>56</v>
       </c>
@@ -1673,16 +1689,16 @@
         <v>105</v>
       </c>
       <c r="C51">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D51">
-        <v>0.0115507330772654</v>
+        <v>1.1550733077265399E-2</v>
       </c>
       <c r="E51">
-        <v>0.0214018834886823</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7">
+        <v>2.14018834886823E-2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>57</v>
       </c>
@@ -1690,13 +1706,13 @@
         <v>106</v>
       </c>
       <c r="C52">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D52">
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:7">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>58</v>
       </c>
@@ -1704,10 +1720,10 @@
         <v>106</v>
       </c>
       <c r="C53">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>59</v>
       </c>
@@ -1715,10 +1731,10 @@
         <v>106</v>
       </c>
       <c r="C54">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>60</v>
       </c>
@@ -1726,22 +1742,22 @@
         <v>106</v>
       </c>
       <c r="C55">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D55">
-        <v>0.0368932758105075</v>
+        <v>3.6893275810507498E-2</v>
       </c>
       <c r="E55">
-        <v>0.0559411721257834</v>
+        <v>5.5941172125783402E-2</v>
       </c>
       <c r="F55">
-        <v>0.06629749362347789</v>
+        <v>6.6297493623477893E-2</v>
       </c>
       <c r="G55">
-        <v>0.1381470541329707</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7">
+        <v>0.13814705413297071</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>61</v>
       </c>
@@ -1749,10 +1765,10 @@
         <v>107</v>
       </c>
       <c r="C56">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>62</v>
       </c>
@@ -1760,22 +1776,22 @@
         <v>107</v>
       </c>
       <c r="C57">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D57">
-        <v>0.0023665483730015</v>
+        <v>2.3665483730014999E-3</v>
       </c>
       <c r="E57">
-        <v>0.0005889834136419</v>
+        <v>5.8898341364189998E-4</v>
       </c>
       <c r="F57">
-        <v>0.0058875360820202</v>
+        <v>5.8875360820202002E-3</v>
       </c>
       <c r="G57">
-        <v>0.0046881752456011</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7">
+        <v>4.6881752456011004E-3</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>63</v>
       </c>
@@ -1783,13 +1799,13 @@
         <v>107</v>
       </c>
       <c r="C58">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D58">
-        <v>0.0948167728070833</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7">
+        <v>9.4816772807083297E-2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>64</v>
       </c>
@@ -1797,22 +1813,22 @@
         <v>107</v>
       </c>
       <c r="C59">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D59">
-        <v>0.0180807169679858</v>
+        <v>1.8080716967985799E-2</v>
       </c>
       <c r="E59">
-        <v>0.0161875795965984</v>
+        <v>1.61875795965984E-2</v>
       </c>
       <c r="F59">
-        <v>0.023589660321911</v>
+        <v>2.3589660321911E-2</v>
       </c>
       <c r="G59">
-        <v>0.0205505096244821</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7">
+        <v>2.05505096244821E-2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>65</v>
       </c>
@@ -1820,22 +1836,22 @@
         <v>108</v>
       </c>
       <c r="C60">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D60">
-        <v>0.0007584161217177</v>
+        <v>7.5841612171769998E-4</v>
       </c>
       <c r="E60">
-        <v>0.0012469202261576</v>
+        <v>1.2469202261575999E-3</v>
       </c>
       <c r="F60">
-        <v>0.0027260662824976</v>
+        <v>2.7260662824976E-3</v>
       </c>
       <c r="G60">
-        <v>0.0020246704439155</v>
-      </c>
-    </row>
-    <row r="61" spans="1:7">
+        <v>2.0246704439155E-3</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>66</v>
       </c>
@@ -1843,22 +1859,22 @@
         <v>108</v>
       </c>
       <c r="C61">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D61">
-        <v>0.009099856377439401</v>
+        <v>9.0998563774394008E-3</v>
       </c>
       <c r="E61">
-        <v>0.0160499513576502</v>
+        <v>1.6049951357650201E-2</v>
       </c>
       <c r="F61">
-        <v>0.0220790595184917</v>
+        <v>2.2079059518491699E-2</v>
       </c>
       <c r="G61">
-        <v>0.0222212087977484</v>
-      </c>
-    </row>
-    <row r="62" spans="1:7">
+        <v>2.2221208797748401E-2</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>67</v>
       </c>
@@ -1866,10 +1882,10 @@
         <v>108</v>
       </c>
       <c r="C62">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="63" spans="1:7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>68</v>
       </c>
@@ -1877,10 +1893,10 @@
         <v>108</v>
       </c>
       <c r="C63">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="64" spans="1:7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>69</v>
       </c>
@@ -1888,22 +1904,22 @@
         <v>109</v>
       </c>
       <c r="C64">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D64">
-        <v>0.0069621446001812</v>
+        <v>6.9621446001811998E-3</v>
       </c>
       <c r="E64">
-        <v>0.0233253766688386</v>
+        <v>2.3325376668838601E-2</v>
       </c>
       <c r="F64">
-        <v>0.0119905319510918</v>
+        <v>1.19905319510918E-2</v>
       </c>
       <c r="G64">
-        <v>0.0150746828217668</v>
-      </c>
-    </row>
-    <row r="65" spans="1:7">
+        <v>1.5074682821766799E-2</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>70</v>
       </c>
@@ -1911,10 +1927,10 @@
         <v>110</v>
       </c>
       <c r="C65">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="66" spans="1:7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>71</v>
       </c>
@@ -1922,22 +1938,22 @@
         <v>110</v>
       </c>
       <c r="C66">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D66">
-        <v>0.0158490691867876</v>
+        <v>1.58490691867876E-2</v>
       </c>
       <c r="E66">
-        <v>0.0106331220896928</v>
+        <v>1.06331220896928E-2</v>
       </c>
       <c r="F66">
-        <v>0.0164797123264719</v>
+        <v>1.6479712326471899E-2</v>
       </c>
       <c r="G66">
-        <v>0.0223997693356085</v>
-      </c>
-    </row>
-    <row r="67" spans="1:7">
+        <v>2.2399769335608499E-2</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>72</v>
       </c>
@@ -1945,19 +1961,19 @@
         <v>110</v>
       </c>
       <c r="C67">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D67">
-        <v>0.057920666800133</v>
+        <v>5.7920666800132997E-2</v>
       </c>
       <c r="E67">
-        <v>0.0235576805016097</v>
+        <v>2.3557680501609699E-2</v>
       </c>
       <c r="F67">
-        <v>0.0165827775003143</v>
-      </c>
-    </row>
-    <row r="68" spans="1:7">
+        <v>1.65827775003143E-2</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>73</v>
       </c>
@@ -1965,10 +1981,10 @@
         <v>110</v>
       </c>
       <c r="C68">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="69" spans="1:7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>74</v>
       </c>
@@ -1976,22 +1992,22 @@
         <v>74</v>
       </c>
       <c r="C69">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D69">
-        <v>0.0541699180160539</v>
+        <v>5.4169918016053899E-2</v>
       </c>
       <c r="E69">
-        <v>0.0142432430866133</v>
+        <v>1.4243243086613301E-2</v>
       </c>
       <c r="F69">
-        <v>0.0463626572757947</v>
+        <v>4.6362657275794701E-2</v>
       </c>
       <c r="G69">
-        <v>0.0300054418769672</v>
-      </c>
-    </row>
-    <row r="70" spans="1:7">
+        <v>3.0005441876967201E-2</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>75</v>
       </c>
@@ -1999,22 +2015,22 @@
         <v>111</v>
       </c>
       <c r="C70">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D70">
-        <v>0.0109883818310779</v>
+        <v>1.0988381831077899E-2</v>
       </c>
       <c r="E70">
-        <v>0.0341985750938111</v>
+        <v>3.41985750938111E-2</v>
       </c>
       <c r="F70">
-        <v>0.0155359153665624</v>
+        <v>1.5535915366562399E-2</v>
       </c>
       <c r="G70">
-        <v>0.019806787566077</v>
-      </c>
-    </row>
-    <row r="71" spans="1:7">
+        <v>1.9806787566077001E-2</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>76</v>
       </c>
@@ -2022,19 +2038,19 @@
         <v>111</v>
       </c>
       <c r="C71">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D71">
-        <v>0.0086701860842934</v>
+        <v>8.6701860842934002E-3</v>
       </c>
       <c r="E71">
-        <v>0.0115478106242526</v>
+        <v>1.15478106242526E-2</v>
       </c>
       <c r="F71">
-        <v>0.0197161510656146</v>
-      </c>
-    </row>
-    <row r="72" spans="1:7">
+        <v>1.9716151065614598E-2</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>77</v>
       </c>
@@ -2042,22 +2058,22 @@
         <v>111</v>
       </c>
       <c r="C72">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D72">
-        <v>0.0236782348016797</v>
+        <v>2.3678234801679701E-2</v>
       </c>
       <c r="E72">
-        <v>0.0314952388829505</v>
+        <v>3.1495238882950499E-2</v>
       </c>
       <c r="F72">
-        <v>0.0170438214927721</v>
+        <v>1.7043821492772102E-2</v>
       </c>
       <c r="G72">
-        <v>0.0214581288922906</v>
-      </c>
-    </row>
-    <row r="73" spans="1:7">
+        <v>2.1458128892290599E-2</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>78</v>
       </c>
@@ -2065,22 +2081,22 @@
         <v>112</v>
       </c>
       <c r="C73">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D73">
         <v>0</v>
       </c>
       <c r="E73">
-        <v>0.013061073134344</v>
+        <v>1.3061073134344001E-2</v>
       </c>
       <c r="F73">
-        <v>0.0035222836964334</v>
+        <v>3.5222836964333998E-3</v>
       </c>
       <c r="G73">
-        <v>0.0021032704602017</v>
-      </c>
-    </row>
-    <row r="74" spans="1:7">
+        <v>2.1032704602017001E-3</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>79</v>
       </c>
@@ -2088,19 +2104,19 @@
         <v>112</v>
       </c>
       <c r="C74">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D74">
-        <v>0.0041468497789956</v>
+        <v>4.1468497789956E-3</v>
       </c>
       <c r="E74">
-        <v>0.0134234456785383</v>
+        <v>1.3423445678538299E-2</v>
       </c>
       <c r="F74">
-        <v>0.0205234786691473</v>
-      </c>
-    </row>
-    <row r="75" spans="1:7">
+        <v>2.0523478669147301E-2</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>80</v>
       </c>
@@ -2108,13 +2124,13 @@
         <v>112</v>
       </c>
       <c r="C75">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D75">
-        <v>0.033232375732994</v>
-      </c>
-    </row>
-    <row r="76" spans="1:7">
+        <v>3.3232375732994E-2</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>81</v>
       </c>
@@ -2122,10 +2138,10 @@
         <v>112</v>
       </c>
       <c r="C76">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="77" spans="1:7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>82</v>
       </c>
@@ -2133,16 +2149,16 @@
         <v>113</v>
       </c>
       <c r="C77">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D77">
-        <v>0.0090803062316911</v>
+        <v>9.0803062316911001E-3</v>
       </c>
       <c r="E77">
-        <v>0.0181987289845117</v>
-      </c>
-    </row>
-    <row r="78" spans="1:7">
+        <v>1.8198728984511699E-2</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>83</v>
       </c>
@@ -2150,19 +2166,19 @@
         <v>113</v>
       </c>
       <c r="C78">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D78">
-        <v>0.0252218618191509</v>
+        <v>2.5221861819150902E-2</v>
       </c>
       <c r="E78">
-        <v>0.0216972734664253</v>
+        <v>2.1697273466425301E-2</v>
       </c>
       <c r="F78">
-        <v>0.0152864804444592</v>
-      </c>
-    </row>
-    <row r="79" spans="1:7">
+        <v>1.52864804444592E-2</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>84</v>
       </c>
@@ -2170,22 +2186,22 @@
         <v>113</v>
       </c>
       <c r="C79">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D79">
         <v>0.1121506047673976</v>
       </c>
       <c r="E79">
-        <v>0.0581565306553574</v>
+        <v>5.8156530655357398E-2</v>
       </c>
       <c r="F79">
-        <v>0.1063351406864839</v>
+        <v>0.10633514068648391</v>
       </c>
       <c r="G79">
-        <v>0.08401884068496231</v>
-      </c>
-    </row>
-    <row r="80" spans="1:7">
+        <v>8.4018840684962307E-2</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>85</v>
       </c>
@@ -2193,10 +2209,10 @@
         <v>113</v>
       </c>
       <c r="C80">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="81" spans="1:7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>86</v>
       </c>
@@ -2204,22 +2220,22 @@
         <v>114</v>
       </c>
       <c r="C81">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D81">
-        <v>0.0663930603623215</v>
+        <v>6.6393060362321496E-2</v>
       </c>
       <c r="E81">
-        <v>0.0380744108860138</v>
+        <v>3.80744108860138E-2</v>
       </c>
       <c r="F81">
-        <v>0.0619202041699453</v>
+        <v>6.19202041699453E-2</v>
       </c>
       <c r="G81">
-        <v>0.0407326745571939</v>
-      </c>
-    </row>
-    <row r="82" spans="1:7">
+        <v>4.0732674557193899E-2</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>87</v>
       </c>
@@ -2227,22 +2243,22 @@
         <v>115</v>
       </c>
       <c r="C82">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D82">
-        <v>0.0960199551544343</v>
+        <v>9.6019955154434303E-2</v>
       </c>
       <c r="E82">
         <v>0.117541031348432</v>
       </c>
       <c r="F82">
-        <v>0.06353377603992361</v>
+        <v>6.3533776039923606E-2</v>
       </c>
       <c r="G82">
-        <v>0.07192137113466029</v>
-      </c>
-    </row>
-    <row r="83" spans="1:7">
+        <v>7.1921371134660295E-2</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>88</v>
       </c>
@@ -2250,24 +2266,24 @@
         <v>116</v>
       </c>
       <c r="C83">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D83">
-        <v>0.0299420232835206</v>
+        <v>2.9942023283520601E-2</v>
       </c>
       <c r="E83">
-        <v>0.01788513796958</v>
+        <v>1.7885137969579998E-2</v>
       </c>
       <c r="F83">
-        <v>0.047091457522531</v>
+        <v>4.7091457522531001E-2</v>
       </c>
       <c r="G83">
-        <v>0.0551360953886155</v>
+        <v>5.5136095388615497E-2</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C83">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C83" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"0,1"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>